<commit_message>
readded model class to the owrkflow
</commit_message>
<xml_diff>
--- a/TradeManager/test/test_data/sellsOnly/TradeRequest.xlsx
+++ b/TradeManager/test/test_data/sellsOnly/TradeRequest.xlsx
@@ -405,7 +405,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -459,6 +461,9 @@
       <c r="D3" s="1">
         <v>98.2</v>
       </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -469,6 +474,9 @@
       </c>
       <c r="D4" s="1">
         <v>74.5</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>